<commit_message>
material link for progress
</commit_message>
<xml_diff>
--- a/examTest.xlsx
+++ b/examTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asaaga\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asaaga\Desktop\CHRISTAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54D02FD-168C-48E0-8EFC-DE20BABFF36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF43102-1CAB-41FF-BC5E-976EB60B1895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" xr2:uid="{4041A3B9-002D-41B1-9B54-9BC69DC3B5DC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>sn</t>
   </si>
@@ -201,15 +201,124 @@
     <t>Atiku Abubakar</t>
   </si>
   <si>
-    <t>opton_b</t>
+    <t>Devices that works once they are connected to computer without necessary installing their drivers are called_____</t>
+  </si>
+  <si>
+    <t>Plug and Play</t>
+  </si>
+  <si>
+    <t>Plug to Play</t>
+  </si>
+  <si>
+    <t>Plug then Play</t>
+  </si>
+  <si>
+    <t>Plug on Play</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The short cut keys for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>align center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is __________</t>
+    </r>
+  </si>
+  <si>
+    <t>ctlr + H</t>
+  </si>
+  <si>
+    <t>ctlr + D</t>
+  </si>
+  <si>
+    <t>ctlr + E</t>
+  </si>
+  <si>
+    <t>ctlr + AE</t>
+  </si>
+  <si>
+    <t>which of the following is not an example of application package</t>
+  </si>
+  <si>
+    <t>DYS-E</t>
+  </si>
+  <si>
+    <t>DBMS</t>
+  </si>
+  <si>
+    <t>MS-DOS</t>
+  </si>
+  <si>
+    <t>spread sheet</t>
+  </si>
+  <si>
+    <t>the egyptian where the people that developed _____as symbols representing words</t>
+  </si>
+  <si>
+    <t>Hieroglyphic</t>
+  </si>
+  <si>
+    <t>alphabeth</t>
+  </si>
+  <si>
+    <t>haeroglyphics</t>
+  </si>
+  <si>
+    <t>algebra</t>
+  </si>
+  <si>
+    <t>the greatest common divisor of 126 and 54 is ______</t>
+  </si>
+  <si>
+    <t>find two numbers such that the arithematic mean is 6.5 and geometric mean is 6</t>
+  </si>
+  <si>
+    <t>3, 6</t>
+  </si>
+  <si>
+    <t>4, 9</t>
+  </si>
+  <si>
+    <t>6,8</t>
+  </si>
+  <si>
+    <t>4, 16</t>
+  </si>
+  <si>
+    <t>if the first and last terms of series are 3 and 35 respectively, find the sum of the first 6 terms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -553,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DE0872-2BBB-420B-9288-B66EB195FDA6}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,19 +709,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -623,22 +732,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -646,22 +755,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -669,22 +778,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -692,19 +801,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>54</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
@@ -715,22 +824,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -738,22 +847,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
+      <c r="D8">
+        <v>76</v>
+      </c>
+      <c r="E8">
+        <v>114</v>
+      </c>
+      <c r="F8">
+        <v>228</v>
       </c>
       <c r="G8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -761,22 +870,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -784,22 +893,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -807,22 +916,183 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F18" t="s">
         <v>57</v>
       </c>
-      <c r="G11" t="s">
-        <v>58</v>
+      <c r="G18" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>